<commit_message>
Update Evaluation Tool and Calculations
</commit_message>
<xml_diff>
--- a/calculos.xlsx
+++ b/calculos.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\GitHub\SIEM-Selection-Methodology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC4CD8F-B4B8-4D31-A27B-4D613E10A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4B7090-B456-4CE1-8E90-9571432E652A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{52376391-DE13-4635-A60B-218E65934C32}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Draft" sheetId="1" r:id="rId1"/>
+    <sheet name="Final Calculations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Quantity</t>
   </si>
@@ -132,9 +132,6 @@
     <t>SIEM Server</t>
   </si>
   <si>
-    <t>SIEM Long term Storage</t>
-  </si>
-  <si>
     <t>SOC Server</t>
   </si>
   <si>
@@ -150,24 +147,12 @@
     <t>SIEM Archive Storage</t>
   </si>
   <si>
-    <t>Domain Server (IAM)</t>
-  </si>
-  <si>
     <t>Included on Applicational Servers</t>
   </si>
   <si>
     <t>Included on SOC Servers</t>
   </si>
   <si>
-    <t>included on Applicational Servers</t>
-  </si>
-  <si>
-    <t>WWW Server</t>
-  </si>
-  <si>
-    <t>Webmail Server</t>
-  </si>
-  <si>
     <t>VPN-GW</t>
   </si>
   <si>
@@ -187,6 +172,33 @@
   </si>
   <si>
     <t>NTP Server</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>WWW and Webmail Server</t>
+  </si>
+  <si>
+    <t>SIEM Long Term Storage</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://tf.nist.gov/general/pdf/2776.pdf</t>
+  </si>
+  <si>
+    <t>https://pitstop.manageengine.com/portal/en/kb/articles/response-rate-limiting-rrl#Configuring_RRL_in_DDI</t>
+  </si>
+  <si>
+    <t>https://documentation.wazuh.com/current/user-manual/agent/agent-management/antiflooding.html</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Total Events per Second</t>
   </si>
 </sst>
 </file>
@@ -196,7 +208,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,19 +243,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF5050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,8 +269,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -284,15 +299,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -632,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B11C34-AF9B-47B6-B0A2-4E3D787FE325}">
   <dimension ref="A2:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -957,24 +973,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656AD650-F90B-4A3F-A50E-360D5093F62D}">
-  <dimension ref="A2:E29"/>
+  <dimension ref="A2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -985,8 +1002,11 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1003,12 +1023,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
@@ -1020,12 +1040,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
@@ -1037,7 +1057,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
@@ -1054,23 +1074,32 @@
         <v>4319</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>7000</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5263</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>21</v>
@@ -1081,13 +1110,16 @@
       <c r="E8" s="4">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -1099,12 +1131,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -1116,79 +1148,105 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>151</v>
-      </c>
-      <c r="E11" s="4">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D12" s="4">
+        <v>172</v>
+      </c>
+      <c r="E12" s="4">
+        <v>130</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>100</v>
+      </c>
+      <c r="E13" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="4">
+        <v>172</v>
+      </c>
+      <c r="E14" s="4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
+      <c r="C16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3">
+        <v>172</v>
+      </c>
+      <c r="E16" s="3">
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1198,6 +1256,15 @@
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="3">
+        <v>172</v>
+      </c>
+      <c r="E17" s="3">
+        <v>130</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1206,141 +1273,129 @@
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>100</v>
+      </c>
+      <c r="E18" s="3">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1380</v>
+      </c>
+      <c r="E19" s="4">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>113</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>3</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="4">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1380</v>
-      </c>
-      <c r="E21" s="4">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>113</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4">
+        <f>SUM(C3:C20)</f>
+        <v>158.6</v>
+      </c>
+      <c r="D23" s="4">
+        <f>SUM(D3:D20)</f>
+        <v>16992</v>
+      </c>
+      <c r="E23" s="4">
+        <f>SUM(E3:E20)</f>
+        <v>11628</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="4">
-        <f>SUM(C3:C21)</f>
-        <v>156.6</v>
-      </c>
-      <c r="D25" s="4">
-        <f>SUM(D3:D21)</f>
-        <v>9255</v>
-      </c>
-      <c r="E25" s="4">
-        <f>SUM(E3:E21)</f>
-        <v>5804</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="B25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="8">
+        <f>(C23*300/1024/1024/1024/1024)*60*60*24</f>
+        <v>3.738852683454752E-3</v>
+      </c>
+      <c r="D25" s="7">
+        <f>(D23*300/1024/1024/1024)*60*60*24/1024</f>
+        <v>0.40057115256786346</v>
+      </c>
+      <c r="E25" s="7">
+        <f>(E23*300/1024/1024/1024/1024)*60*60*24</f>
+        <v>0.2741196658462286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="8">
+        <f>C25*31</f>
+        <v>0.11590443318709731</v>
+      </c>
+      <c r="D26" s="7">
+        <f>D25*31</f>
+        <v>12.417705729603767</v>
+      </c>
+      <c r="E26" s="7">
+        <f>E25*31</f>
+        <v>8.4977096412330866</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C27" s="8">
-        <f>(C25*300/1024/1024/1024)*60*60*24/1024</f>
-        <v>3.6917044781148434E-3</v>
+        <f>C25*365</f>
+        <v>1.3646812294609845</v>
       </c>
       <c r="D27" s="7">
-        <f>(D25*300/1024/1024/1024)*60*60*24/1024</f>
-        <v>0.21817832021042705</v>
+        <f>D25*365</f>
+        <v>146.20847068727016</v>
       </c>
       <c r="E27" s="7">
-        <f>(E25*300/1024/1024/1024)*60*60*24/1024</f>
-        <v>0.13682409189641476</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="8">
-        <f>C27*31</f>
-        <v>0.11444283882156014</v>
-      </c>
-      <c r="D28" s="7">
-        <f>D27*31</f>
-        <v>6.7635279265232384</v>
-      </c>
-      <c r="E28" s="7">
-        <f>E27*31</f>
-        <v>4.2415468487888575</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="8">
-        <f>C27*365</f>
-        <v>1.3474721345119178</v>
-      </c>
-      <c r="D29" s="7">
-        <f>D27*365</f>
-        <v>79.635086876805872</v>
-      </c>
-      <c r="E29" s="7">
-        <f>E27*365</f>
-        <v>49.940793542191386</v>
+        <f>E25*365</f>
+        <v>100.05367803387344</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C15:E15"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{9854F2A5-BF19-4B51-8A04-B53D7368CC16}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>